<commit_message>
updated carry marks files
</commit_message>
<xml_diff>
--- a/OGA_STA404.xlsx
+++ b/OGA_STA404.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F173796-2218-47C3-99E6-73E4064F41AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF64AD83-1E8B-4594-A2D8-46AE2CB03859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BAC27743-BA74-45ED-A773-A10367CAE196}"/>
   </bookViews>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465C901A-2E30-4458-B3F9-38E1A2BAB49E}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
@@ -721,13 +721,15 @@
       <c r="D7" s="5">
         <v>8</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="5">
+        <v>11</v>
+      </c>
       <c r="F7" s="5">
         <v>48</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="0"/>
-        <v>21.866666666666667</v>
+        <v>28.466666666666665</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -809,13 +811,15 @@
       <c r="D11" s="5">
         <v>5</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="5">
+        <v>23.5</v>
+      </c>
       <c r="F11" s="5">
         <v>42.75</v>
       </c>
       <c r="G11" s="6">
         <f t="shared" si="0"/>
-        <v>18.766666666666669</v>
+        <v>32.866666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -1029,13 +1033,15 @@
       <c r="D21" s="5">
         <v>10</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="5">
+        <v>23</v>
+      </c>
       <c r="F21" s="5">
         <v>27</v>
       </c>
       <c r="G21" s="6">
         <f t="shared" si="0"/>
-        <v>14.133333333333333</v>
+        <v>27.933333333333334</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
@@ -1073,13 +1079,15 @@
       <c r="D23" s="5">
         <v>12.5</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="5">
+        <v>26</v>
+      </c>
       <c r="F23" s="5">
         <v>43.25</v>
       </c>
       <c r="G23" s="6">
         <f t="shared" si="0"/>
-        <v>21.466666666666669</v>
+        <v>37.06666666666667</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">

</xml_diff>